<commit_message>
Added updated xlsx to find model that gives min metric
</commit_message>
<xml_diff>
--- a/metrics.xlsx
+++ b/metrics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nimda/Desktop/Programs/Python/CS334/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0196095-8C5D-814E-AE0B-74D07AF6CE35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59066C68-6D10-1A44-96AA-F9CFA6ABED67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" activeTab="4" xr2:uid="{AD7D65D4-DA30-7645-8292-FC325879A194}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{AD7D65D4-DA30-7645-8292-FC325879A194}"/>
   </bookViews>
   <sheets>
     <sheet name="Metrics" sheetId="1" r:id="rId1"/>
@@ -19,15 +19,7 @@
     <sheet name="MAPE" sheetId="4" r:id="rId4"/>
     <sheet name="R^2" sheetId="5" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">(Metrics!$B$5:$B$10,Metrics!$H$5:$H$10)</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">(Metrics!$F$5:$F$10,Metrics!$L$5:$L$10)</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Metrics!$F$4</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">(Metrics!$B$5:$B$10,Metrics!$H$5:$H$10)</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">(Metrics!$F$5:$F$10,Metrics!$L$5:$L$10)</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Metrics!$F$4</definedName>
-  </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,6 +35,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -284,10 +298,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>(Metrics!$D$5:$D$10,Metrics!$J$6:$J$10)</c:f>
+              <c:f>(Metrics!$D$5:$D$10,Metrics!$J$6:$J$10,Metrics!$J$5)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>7.7191132358000001</c:v>
                 </c:pt>
@@ -320,6 +334,9 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>12.921336776189399</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>7.71765959422995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3728,7 +3745,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{225BC05B-3994-194A-830E-D0E92C23B409}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="128" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4164,10 +4181,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46E7599B-D00C-C24D-8311-3C56F02D1434}">
-  <dimension ref="B3:L11"/>
+  <dimension ref="B3:L12"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4413,6 +4430,40 @@
     <row r="11" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
     </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="C12" t="str" cm="1">
+        <f t="array" aca="1" ref="C12" ca="1">CELL("address",INDEX(C5:C10,MATCH(MIN(C5:C10),C5:C10,0)))</f>
+        <v>$C$6</v>
+      </c>
+      <c r="D12" t="str" cm="1">
+        <f t="array" aca="1" ref="D12" ca="1">CELL("address",INDEX(D5:D10,MATCH(MIN(D5:D10),D5:D10,0)))</f>
+        <v>$D$5</v>
+      </c>
+      <c r="E12" t="str" cm="1">
+        <f t="array" aca="1" ref="E12" ca="1">CELL("address",INDEX(E5:E10,MATCH(MIN(E5:E10),E5:E10,0)))</f>
+        <v>$E$5</v>
+      </c>
+      <c r="F12" t="str" cm="1">
+        <f t="array" aca="1" ref="F12" ca="1">CELL("address",INDEX(F5:F10,MATCH(MIN(F5:F10),F5:F10,0)))</f>
+        <v>$F$10</v>
+      </c>
+      <c r="I12" t="str" cm="1">
+        <f t="array" aca="1" ref="I12" ca="1">CELL("address",INDEX(I5:I10,MATCH(MIN(I5:I10),I5:I10,0)))</f>
+        <v>$I$6</v>
+      </c>
+      <c r="J12" t="str" cm="1">
+        <f t="array" aca="1" ref="J12" ca="1">CELL("address",INDEX(J5:J10,MATCH(MIN(J5:J10),J5:J10,0)))</f>
+        <v>$J$9</v>
+      </c>
+      <c r="K12" t="str" cm="1">
+        <f t="array" aca="1" ref="K12" ca="1">CELL("address",INDEX(K5:K10,MATCH(MIN(K5:K10),K5:K10,0)))</f>
+        <v>$K$7</v>
+      </c>
+      <c r="L12" t="str" cm="1">
+        <f t="array" aca="1" ref="L12" ca="1">CELL("address",INDEX(L5:L10,MATCH(MIN(L5:L10),L5:L10,0)))</f>
+        <v>$L$10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>